<commit_message>
opgeschoond voor het opsturen naar Pascal
</commit_message>
<xml_diff>
--- a/ArduinoCodePrakticumEE21_opdracht3b_met_display/Doumenten/LDR Meeting.xlsx
+++ b/ArduinoCodePrakticumEE21_opdracht3b_met_display/Doumenten/LDR Meeting.xlsx
@@ -190,10 +190,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,11 +425,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="218287872"/>
-        <c:axId val="354598336"/>
+        <c:axId val="166562816"/>
+        <c:axId val="166563376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="218287872"/>
+        <c:axId val="166562816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,7 +472,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354598336"/>
+        <c:crossAx val="166563376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -473,7 +480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="354598336"/>
+        <c:axId val="166563376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -512,7 +519,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218287872"/>
+        <c:crossAx val="166562816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1452,18 +1459,18 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1505,7 +1512,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
@@ -1546,7 +1553,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -1587,60 +1594,60 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1">
-        <f>B2-B3</f>
+        <f t="shared" ref="B5:M5" si="0">B2-B3</f>
         <v>3.7</v>
       </c>
       <c r="C5" s="1">
-        <f>C2-C3</f>
+        <f t="shared" si="0"/>
         <v>3.7329999999999997</v>
       </c>
       <c r="D5" s="1">
-        <f>D2-D3</f>
+        <f t="shared" si="0"/>
         <v>4.5469999999999997</v>
       </c>
       <c r="E5" s="1">
-        <f>E2-E3</f>
+        <f t="shared" si="0"/>
         <v>4.843</v>
       </c>
       <c r="F5" s="1">
-        <f>F2-F3</f>
+        <f t="shared" si="0"/>
         <v>4.8970000000000002</v>
       </c>
       <c r="G5" s="1">
-        <f>G2-G3</f>
+        <f t="shared" si="0"/>
         <v>4.9110000000000005</v>
       </c>
       <c r="H5" s="1">
-        <f>H2-H3</f>
+        <f t="shared" si="0"/>
         <v>4.92</v>
       </c>
       <c r="I5" s="1">
-        <f>I2-I3</f>
+        <f t="shared" si="0"/>
         <v>4.9279999999999999</v>
       </c>
       <c r="J5" s="1">
-        <f>J2-J3</f>
+        <f t="shared" si="0"/>
         <v>4.9729999999999999</v>
       </c>
       <c r="K5" s="1">
-        <f>K2-K3</f>
+        <f t="shared" si="0"/>
         <v>4.9020000000000001</v>
       </c>
       <c r="L5" s="1">
-        <f>L2-L3</f>
+        <f t="shared" si="0"/>
         <v>4.88</v>
       </c>
       <c r="M5" s="1">
-        <f>M2-M3</f>
+        <f t="shared" si="0"/>
         <v>4.8140000000000001</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J17" s="2"/>
+      <c r="J17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>